<commit_message>
finish 6th step of cleaning
</commit_message>
<xml_diff>
--- a/Reduction of ketone/experiment_to_test/commercial_available_positive.xlsx
+++ b/Reduction of ketone/experiment_to_test/commercial_available_positive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suongsuong/Documents/GitHub/Reactivity-based-metric-of-complexity/Reduction of ketone/experiment_to_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0D13A8-C28F-9541-AFD9-D952E1548FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03F5E2E-148B-7540-BA15-10B0AFAE115E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="16780" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>wendlandt</t>
   </si>
   <si>
-    <t>To a solution of Wieland-Miescher ketone (1.0 g, 5.6 mmol) exhibiting (a], + 100 (c 1.0, toluene) in methanol (30 mL) at 0°C was added, dropwise, a solution of NaBH, (0.14 g, 3.7 mmol) in methanol (20 mL). The solution was stirred at 0°C for 30 min and several drops of acetic acid were added. The mixture was concentrated under vacuum, water was added, and the product was extracted into ether (3 X 20 mL), dried, concentrated, and purified by flash chromatography (elution with 30% ethyl acetate in petroleum ether) to give 0.980 g (97%) of the 2ß-ol-S-one as a colorless oil; [al + 183 (c 1.7, CHCl); ir (CHCl,): 3600, 3450, 1665, and 1620 cm'; 'H mr (300 MHz, CDCl;) &amp;; 5.73 (s, 1H), 3.37</t>
-  </si>
-  <si>
     <t>https://www.reaxys.com/reaxys/secured/hopinto.do?context=C&amp;query=CNR.CNR%3D5707398&amp;database=RX&amp;origin=ReaxysOutput&amp;ln=</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>403-42-9</t>
+  </si>
+  <si>
+    <t>To a solution of Wieland-Miescher ketone (1.0 g, 5.6 mmol) exhibiting (a], + 100 (c 1.0, toluene) in methanol (30 mL) at 0°C was added, dropwise, a solution of NaBH, (0.14 g, 3.7 mmol) in methanol (20 mL). The solution was stirred at 0°C for 30 min and several drops of acetic acid were added. The mixture was concentrated under vacuum, water was added, and the product was extracted into ether (3 X 20 mL), dried, concentrated, and purified by flash chromatography (elution with 30% ethyl acetate in petroleum ether) to give 0.980 g (97%) of the 2ß-ol-S-one as a colorless oil; [al + 183 (c 1.7, CHCl); ir (CHCl,): 3600, 3450, 1665, and 1620 cm'; 'H mr (300 MHz, CDCl;) &amp;; 5.73 (s, 1H), 3.37 (dd, J = 1 1.5, 4.4 Hz, 1 H), 2.66 (br s, lH), 2.45-2.10 (series of m, 6H), 1.82 (m, 2H), 1.64 (m, IH), 1.45 (m, lH), 1.15 (s, 3H); I3c nrnr (75 MHz, CDCl,): 199.84, 169.04, 125.17, 77.95, 41.58, 34.10, 33.59, 31.96, 30.09, 23.08, 15.19 ppm; ms m/z (M+) calcd.: 180.1 150; found: 180.1 167.</t>
   </si>
 </sst>
 </file>
@@ -677,12 +677,13 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="52.5" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -756,13 +757,13 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F4">
         <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -770,19 +771,19 @@
         <v>997369</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>98</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -790,19 +791,19 @@
         <v>759034</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6">
         <v>98</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -810,19 +811,19 @@
         <v>1563771</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7">
         <v>90</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -830,19 +831,19 @@
         <v>578384</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>